<commit_message>
update data of httpd
</commit_message>
<xml_diff>
--- a/results/result.xlsx
+++ b/results/result.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="69">
   <si>
     <t xml:space="preserve">lto</t>
   </si>
@@ -96,6 +96,9 @@
     <t xml:space="preserve">max multi tag</t>
   </si>
   <si>
+    <t xml:space="preserve">Max length</t>
+  </si>
+  <si>
     <t xml:space="preserve">original size</t>
   </si>
   <si>
@@ -208,6 +211,18 @@
   </si>
   <si>
     <t xml:space="preserve">444.namd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">httpd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{0: 40, 1: 13}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{0: 216, 1: 155}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{0: 220, 1: 13}</t>
   </si>
   <si>
     <t xml:space="preserve">./baseline.:</t>
@@ -345,10 +360,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,23 +661,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.984693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.4591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -690,19 +707,22 @@
       <c r="I1" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>24</v>
+      </c>
       <c r="K1" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>413</v>
@@ -717,16 +737,19 @@
         <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>6</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>1064757</v>
@@ -741,7 +764,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>23</v>
@@ -756,15 +779,18 @@
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K3" s="0" t="n">
@@ -780,7 +806,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>367</v>
@@ -795,16 +821,19 @@
         <v>43</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>7</v>
       </c>
       <c r="K4" s="0" t="n">
         <v>2959541</v>
@@ -819,7 +848,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>40</v>
@@ -834,16 +863,19 @@
         <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>696117</v>
@@ -858,7 +890,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>12</v>
@@ -873,15 +905,18 @@
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K6" s="0" t="n">
@@ -897,7 +932,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
@@ -912,15 +947,18 @@
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="I7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K7" s="0" t="n">
@@ -936,7 +974,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>367</v>
@@ -951,16 +989,19 @@
         <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>523157</v>
@@ -975,7 +1016,7 @@
     </row>
     <row r="9" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>2020</v>
@@ -990,18 +1031,20 @@
         <v>124</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I9" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="J9" s="4"/>
+      <c r="J9" s="4" t="n">
+        <v>8</v>
+      </c>
       <c r="K9" s="4" t="n">
         <v>645541</v>
       </c>
@@ -1015,7 +1058,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B10" s="4" t="n">
         <v>1</v>
@@ -1030,18 +1073,20 @@
         <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I10" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J10" s="4"/>
+      <c r="J10" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="K10" s="4" t="n">
         <v>30437</v>
       </c>
@@ -1055,7 +1100,7 @@
     </row>
     <row r="11" customFormat="false" ht="58.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B11" s="3" t="n">
         <v>20038</v>
@@ -1070,18 +1115,20 @@
         <v>807</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I11" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="J11" s="4"/>
+      <c r="J11" s="4" t="n">
+        <v>7</v>
+      </c>
       <c r="K11" s="4" t="n">
         <v>2387189</v>
       </c>
@@ -1100,7 +1147,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>82245</v>
@@ -1111,13 +1158,45 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K16" s="0" t="n">
         <v>236293</v>
       </c>
       <c r="L16" s="0" t="n">
         <v>236389</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>398</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>233</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>371</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1138,27 +1217,29 @@
   </sheetPr>
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="13" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>62</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="B1" s="0"/>
+      <c r="N1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>426.140889</v>
@@ -1197,10 +1278,11 @@
         <f aca="false">AVERAGE(C2:L2)</f>
         <v>464.5333037</v>
       </c>
+      <c r="N2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>431.97578</v>
@@ -1239,10 +1321,11 @@
         <f aca="false">AVERAGE(C3:L3)</f>
         <v>428.3123397</v>
       </c>
+      <c r="N3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" s="4" t="n">
         <v>339.981264</v>
@@ -1281,10 +1364,11 @@
         <f aca="false">AVERAGE(C4:L4)</f>
         <v>306.2730011</v>
       </c>
+      <c r="N4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>218.007827</v>
@@ -1323,10 +1407,11 @@
         <f aca="false">AVERAGE(C5:L5)</f>
         <v>253.4190938</v>
       </c>
+      <c r="N5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>319.2761</v>
@@ -1365,10 +1450,11 @@
         <f aca="false">AVERAGE(C6:L6)</f>
         <v>311.2826534</v>
       </c>
+      <c r="N6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>327.955631</v>
@@ -1407,10 +1493,11 @@
         <f aca="false">AVERAGE(C7:L7)</f>
         <v>328.3348524</v>
       </c>
+      <c r="N7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B8" s="4" t="n">
         <v>451.953723</v>
@@ -1449,10 +1536,11 @@
         <f aca="false">AVERAGE(C8:L8)</f>
         <v>472.2218224</v>
       </c>
+      <c r="N8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9" s="4" t="n">
         <v>461.860597</v>
@@ -1491,10 +1579,11 @@
         <f aca="false">AVERAGE(C9:L9)</f>
         <v>480.2210457</v>
       </c>
+      <c r="N9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B10" s="4" t="n">
         <v>354.837712</v>
@@ -1533,10 +1622,11 @@
         <f aca="false">AVERAGE(C10:L10)</f>
         <v>360.7686142</v>
       </c>
+      <c r="N10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11" s="4" t="n">
         <v>385.199008</v>
@@ -1575,10 +1665,11 @@
         <f aca="false">AVERAGE(C11:L11)</f>
         <v>382.5664891</v>
       </c>
+      <c r="N11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B12" s="4" t="n">
         <v>179.78234</v>
@@ -1617,10 +1708,11 @@
         <f aca="false">AVERAGE(C12:L12)</f>
         <v>198.326745</v>
       </c>
+      <c r="N12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B13" s="4" t="n">
         <v>335.815794</v>
@@ -1659,15 +1751,18 @@
         <f aca="false">AVERAGE(C13:L13)</f>
         <v>318.9990819</v>
       </c>
+      <c r="N13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>63</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="B14" s="0"/>
+      <c r="N14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" s="4" t="n">
         <v>445.817547</v>
@@ -1713,7 +1808,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" s="4" t="n">
         <v>453.757756</v>
@@ -1759,7 +1854,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" s="4" t="n">
         <v>285.555329</v>
@@ -1805,7 +1900,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="4" t="n">
         <v>233.008332</v>
@@ -1851,7 +1946,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B19" s="4" t="n">
         <v>332.631266</v>
@@ -1897,7 +1992,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B20" s="4" t="n">
         <v>393.485039</v>
@@ -1943,7 +2038,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B21" s="4" t="n">
         <v>454.269451</v>
@@ -1989,7 +2084,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" s="4" t="n">
         <v>480.910419</v>
@@ -2035,7 +2130,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B23" s="4" t="n">
         <v>355.322246</v>
@@ -2081,7 +2176,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B24" s="4" t="n">
         <v>360.83511</v>
@@ -2127,7 +2222,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B25" s="4" t="n">
         <v>269.156459</v>
@@ -2173,7 +2268,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B26" s="4" t="n">
         <v>334.201438</v>

</xml_diff>